<commit_message>
Subscript BVTQaZ and VTQaZ by Vehicle Type
</commit_message>
<xml_diff>
--- a/InputData/trans/BVTQaZ/BAU Veh Techs Qualifying as ZEVs.xlsx
+++ b/InputData/trans/BVTQaZ/BAU Veh Techs Qualifying as ZEVs.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\BVTQaZ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\trans\BVTQaZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491C0F1E-D394-4C20-8581-8BA4404F7540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D6E708-877B-4EA5-8B13-7CB340C7CC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="6405" windowWidth="28800" windowHeight="15600" xr2:uid="{7166B4F5-29DF-47A7-8501-7E54D22AC689}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{7166B4F5-29DF-47A7-8501-7E54D22AC689}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="BVTQaZ" sheetId="2" r:id="rId2"/>
+    <sheet name="BVTQaZ-LDVs" sheetId="2" r:id="rId2"/>
+    <sheet name="BVTQaZ-HDVs" sheetId="7" r:id="rId3"/>
+    <sheet name="BVTQaZ-aircraft" sheetId="6" r:id="rId4"/>
+    <sheet name="BVTQaZ-rail" sheetId="5" r:id="rId5"/>
+    <sheet name="BVTQaZ-ships" sheetId="4" r:id="rId6"/>
+    <sheet name="BVTQaZ-motorbikes" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="11">
   <si>
     <t>Source:</t>
   </si>
@@ -143,9 +148,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -183,7 +188,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -289,7 +294,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -431,7 +436,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -473,8 +478,8 @@
   </sheetPr>
   <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AE16" sqref="AE16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,4 +1274,4029 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EDCB297-CFBF-40EF-B9D6-01AA1938CA73}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:AF8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>2020</v>
+      </c>
+      <c r="C1">
+        <v>2021</v>
+      </c>
+      <c r="D1">
+        <v>2022</v>
+      </c>
+      <c r="E1">
+        <v>2023</v>
+      </c>
+      <c r="F1">
+        <v>2024</v>
+      </c>
+      <c r="G1">
+        <v>2025</v>
+      </c>
+      <c r="H1">
+        <v>2026</v>
+      </c>
+      <c r="I1">
+        <v>2027</v>
+      </c>
+      <c r="J1">
+        <v>2028</v>
+      </c>
+      <c r="K1">
+        <v>2029</v>
+      </c>
+      <c r="L1">
+        <v>2030</v>
+      </c>
+      <c r="M1">
+        <v>2031</v>
+      </c>
+      <c r="N1">
+        <v>2032</v>
+      </c>
+      <c r="O1">
+        <v>2033</v>
+      </c>
+      <c r="P1">
+        <v>2034</v>
+      </c>
+      <c r="Q1">
+        <v>2035</v>
+      </c>
+      <c r="R1">
+        <v>2036</v>
+      </c>
+      <c r="S1">
+        <v>2037</v>
+      </c>
+      <c r="T1">
+        <v>2038</v>
+      </c>
+      <c r="U1">
+        <v>2039</v>
+      </c>
+      <c r="V1">
+        <v>2040</v>
+      </c>
+      <c r="W1">
+        <v>2041</v>
+      </c>
+      <c r="X1">
+        <v>2042</v>
+      </c>
+      <c r="Y1">
+        <v>2043</v>
+      </c>
+      <c r="Z1">
+        <v>2044</v>
+      </c>
+      <c r="AA1">
+        <v>2045</v>
+      </c>
+      <c r="AB1">
+        <v>2046</v>
+      </c>
+      <c r="AC1">
+        <v>2047</v>
+      </c>
+      <c r="AD1">
+        <v>2048</v>
+      </c>
+      <c r="AE1">
+        <v>2049</v>
+      </c>
+      <c r="AF1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817B9AE7-400E-42A1-A658-6C93FFA8A311}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:AF8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>2020</v>
+      </c>
+      <c r="C1">
+        <v>2021</v>
+      </c>
+      <c r="D1">
+        <v>2022</v>
+      </c>
+      <c r="E1">
+        <v>2023</v>
+      </c>
+      <c r="F1">
+        <v>2024</v>
+      </c>
+      <c r="G1">
+        <v>2025</v>
+      </c>
+      <c r="H1">
+        <v>2026</v>
+      </c>
+      <c r="I1">
+        <v>2027</v>
+      </c>
+      <c r="J1">
+        <v>2028</v>
+      </c>
+      <c r="K1">
+        <v>2029</v>
+      </c>
+      <c r="L1">
+        <v>2030</v>
+      </c>
+      <c r="M1">
+        <v>2031</v>
+      </c>
+      <c r="N1">
+        <v>2032</v>
+      </c>
+      <c r="O1">
+        <v>2033</v>
+      </c>
+      <c r="P1">
+        <v>2034</v>
+      </c>
+      <c r="Q1">
+        <v>2035</v>
+      </c>
+      <c r="R1">
+        <v>2036</v>
+      </c>
+      <c r="S1">
+        <v>2037</v>
+      </c>
+      <c r="T1">
+        <v>2038</v>
+      </c>
+      <c r="U1">
+        <v>2039</v>
+      </c>
+      <c r="V1">
+        <v>2040</v>
+      </c>
+      <c r="W1">
+        <v>2041</v>
+      </c>
+      <c r="X1">
+        <v>2042</v>
+      </c>
+      <c r="Y1">
+        <v>2043</v>
+      </c>
+      <c r="Z1">
+        <v>2044</v>
+      </c>
+      <c r="AA1">
+        <v>2045</v>
+      </c>
+      <c r="AB1">
+        <v>2046</v>
+      </c>
+      <c r="AC1">
+        <v>2047</v>
+      </c>
+      <c r="AD1">
+        <v>2048</v>
+      </c>
+      <c r="AE1">
+        <v>2049</v>
+      </c>
+      <c r="AF1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29612E15-1C93-4627-843E-8219C3220F67}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:AF8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>2020</v>
+      </c>
+      <c r="C1">
+        <v>2021</v>
+      </c>
+      <c r="D1">
+        <v>2022</v>
+      </c>
+      <c r="E1">
+        <v>2023</v>
+      </c>
+      <c r="F1">
+        <v>2024</v>
+      </c>
+      <c r="G1">
+        <v>2025</v>
+      </c>
+      <c r="H1">
+        <v>2026</v>
+      </c>
+      <c r="I1">
+        <v>2027</v>
+      </c>
+      <c r="J1">
+        <v>2028</v>
+      </c>
+      <c r="K1">
+        <v>2029</v>
+      </c>
+      <c r="L1">
+        <v>2030</v>
+      </c>
+      <c r="M1">
+        <v>2031</v>
+      </c>
+      <c r="N1">
+        <v>2032</v>
+      </c>
+      <c r="O1">
+        <v>2033</v>
+      </c>
+      <c r="P1">
+        <v>2034</v>
+      </c>
+      <c r="Q1">
+        <v>2035</v>
+      </c>
+      <c r="R1">
+        <v>2036</v>
+      </c>
+      <c r="S1">
+        <v>2037</v>
+      </c>
+      <c r="T1">
+        <v>2038</v>
+      </c>
+      <c r="U1">
+        <v>2039</v>
+      </c>
+      <c r="V1">
+        <v>2040</v>
+      </c>
+      <c r="W1">
+        <v>2041</v>
+      </c>
+      <c r="X1">
+        <v>2042</v>
+      </c>
+      <c r="Y1">
+        <v>2043</v>
+      </c>
+      <c r="Z1">
+        <v>2044</v>
+      </c>
+      <c r="AA1">
+        <v>2045</v>
+      </c>
+      <c r="AB1">
+        <v>2046</v>
+      </c>
+      <c r="AC1">
+        <v>2047</v>
+      </c>
+      <c r="AD1">
+        <v>2048</v>
+      </c>
+      <c r="AE1">
+        <v>2049</v>
+      </c>
+      <c r="AF1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7727D32E-5813-40B0-A843-07A3A5963E91}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:AF8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>2020</v>
+      </c>
+      <c r="C1">
+        <v>2021</v>
+      </c>
+      <c r="D1">
+        <v>2022</v>
+      </c>
+      <c r="E1">
+        <v>2023</v>
+      </c>
+      <c r="F1">
+        <v>2024</v>
+      </c>
+      <c r="G1">
+        <v>2025</v>
+      </c>
+      <c r="H1">
+        <v>2026</v>
+      </c>
+      <c r="I1">
+        <v>2027</v>
+      </c>
+      <c r="J1">
+        <v>2028</v>
+      </c>
+      <c r="K1">
+        <v>2029</v>
+      </c>
+      <c r="L1">
+        <v>2030</v>
+      </c>
+      <c r="M1">
+        <v>2031</v>
+      </c>
+      <c r="N1">
+        <v>2032</v>
+      </c>
+      <c r="O1">
+        <v>2033</v>
+      </c>
+      <c r="P1">
+        <v>2034</v>
+      </c>
+      <c r="Q1">
+        <v>2035</v>
+      </c>
+      <c r="R1">
+        <v>2036</v>
+      </c>
+      <c r="S1">
+        <v>2037</v>
+      </c>
+      <c r="T1">
+        <v>2038</v>
+      </c>
+      <c r="U1">
+        <v>2039</v>
+      </c>
+      <c r="V1">
+        <v>2040</v>
+      </c>
+      <c r="W1">
+        <v>2041</v>
+      </c>
+      <c r="X1">
+        <v>2042</v>
+      </c>
+      <c r="Y1">
+        <v>2043</v>
+      </c>
+      <c r="Z1">
+        <v>2044</v>
+      </c>
+      <c r="AA1">
+        <v>2045</v>
+      </c>
+      <c r="AB1">
+        <v>2046</v>
+      </c>
+      <c r="AC1">
+        <v>2047</v>
+      </c>
+      <c r="AD1">
+        <v>2048</v>
+      </c>
+      <c r="AE1">
+        <v>2049</v>
+      </c>
+      <c r="AF1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C59BC70-DB17-41C6-993A-0AB202F22A99}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:AF8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>2020</v>
+      </c>
+      <c r="C1">
+        <v>2021</v>
+      </c>
+      <c r="D1">
+        <v>2022</v>
+      </c>
+      <c r="E1">
+        <v>2023</v>
+      </c>
+      <c r="F1">
+        <v>2024</v>
+      </c>
+      <c r="G1">
+        <v>2025</v>
+      </c>
+      <c r="H1">
+        <v>2026</v>
+      </c>
+      <c r="I1">
+        <v>2027</v>
+      </c>
+      <c r="J1">
+        <v>2028</v>
+      </c>
+      <c r="K1">
+        <v>2029</v>
+      </c>
+      <c r="L1">
+        <v>2030</v>
+      </c>
+      <c r="M1">
+        <v>2031</v>
+      </c>
+      <c r="N1">
+        <v>2032</v>
+      </c>
+      <c r="O1">
+        <v>2033</v>
+      </c>
+      <c r="P1">
+        <v>2034</v>
+      </c>
+      <c r="Q1">
+        <v>2035</v>
+      </c>
+      <c r="R1">
+        <v>2036</v>
+      </c>
+      <c r="S1">
+        <v>2037</v>
+      </c>
+      <c r="T1">
+        <v>2038</v>
+      </c>
+      <c r="U1">
+        <v>2039</v>
+      </c>
+      <c r="V1">
+        <v>2040</v>
+      </c>
+      <c r="W1">
+        <v>2041</v>
+      </c>
+      <c r="X1">
+        <v>2042</v>
+      </c>
+      <c r="Y1">
+        <v>2043</v>
+      </c>
+      <c r="Z1">
+        <v>2044</v>
+      </c>
+      <c r="AA1">
+        <v>2045</v>
+      </c>
+      <c r="AB1">
+        <v>2046</v>
+      </c>
+      <c r="AC1">
+        <v>2047</v>
+      </c>
+      <c r="AD1">
+        <v>2048</v>
+      </c>
+      <c r="AE1">
+        <v>2049</v>
+      </c>
+      <c r="AF1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>